<commit_message>
Acrescentado o backend Xeno
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -1,65 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a149c0897170507f/Documentos/GitHub/VelocidadeInternet/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_8B7E81778366F20F6235547658668EBFAEDABEA0" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{EEBF17D7-9B74-450A-A6A7-CCFB7C2F0C1F}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="14595" yWindow="2400" windowWidth="9300" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="base" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="base" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>Data</t>
-  </si>
-  <si>
-    <t>Hora</t>
-  </si>
-  <si>
-    <t>Velocidade</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -74,44 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -399,34 +420,172 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D6" s="2"/>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Data</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Hora</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Velocidade</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>05/04/2021</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>00:11</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>05/04/2021</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>00:12</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>05/04/2021</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>00:12</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>05/04/2021</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>00:24</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>05/04/2021</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>00:24</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>05/04/2021</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>00:25</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>05/04/2021</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>00:26</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>05/04/2021</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>00:26</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>05/04/2021</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>00:27</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>58</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>